<commit_message>
Updating the simulation spread
</commit_message>
<xml_diff>
--- a/python/xlsx/Simulation_Spread.xlsx
+++ b/python/xlsx/Simulation_Spread.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ericp\OneDrive - McGill University\Classes\MGSC 640 - Fundamentals of Decision Analytics\Group Project\dev\python\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="77" documentId="8_{6C55C3BE-0F6E-4149-8734-1B3DF3377D4A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{A5D6635B-CC58-4CE6-AF82-4FF8F694C1E9}"/>
+  <xr:revisionPtr revIDLastSave="86" documentId="8_{6C55C3BE-0F6E-4149-8734-1B3DF3377D4A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{18906C6E-35EC-45D4-98D2-68B2F81D2FE9}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{5D6DE6A9-DCDC-4B30-A344-6E79435D6AEB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0" concurrentManualCount="4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -55,7 +55,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,15 +97,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -410,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB0F30CA-25BB-4F74-B902-CE4726E3E9BF}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="M12" sqref="M11:M12"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -421,7 +431,7 @@
     <col min="8" max="8" width="20.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>5</v>
       </c>
@@ -441,21 +451,21 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>-10</v>
       </c>
       <c r="B2">
         <f t="shared" ref="B2:B10" si="0">1-SUM(C2:D2)</f>
-        <v>0.65000000000000013</v>
+        <v>0.88</v>
       </c>
       <c r="C2">
         <f t="shared" ref="C2:C11" si="1">C3-($G$2)</f>
-        <v>0.29999999999999982</v>
+        <v>0.11</v>
       </c>
       <c r="D2">
         <f t="shared" ref="D2:D11" si="2">D3-$G$2</f>
-        <v>5.0000000000000044E-2</v>
+        <v>1.0000000000000002E-2</v>
       </c>
       <c r="F2" t="s">
         <v>3</v>
@@ -464,375 +474,441 @@
         <v>0.02</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>-9</v>
       </c>
       <c r="B3">
         <f t="shared" si="0"/>
-        <v>0.6100000000000001</v>
+        <v>0.84</v>
       </c>
       <c r="C3">
         <f t="shared" si="1"/>
-        <v>0.31999999999999984</v>
+        <v>0.13</v>
       </c>
       <c r="D3">
         <f t="shared" si="2"/>
-        <v>7.0000000000000048E-2</v>
+        <v>3.0000000000000002E-2</v>
       </c>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>-8</v>
       </c>
       <c r="B4">
-        <f t="shared" si="0"/>
-        <v>0.57000000000000006</v>
+        <v>0.8</v>
       </c>
       <c r="C4">
-        <f t="shared" si="1"/>
-        <v>0.33999999999999986</v>
+        <v>0.15</v>
       </c>
       <c r="D4">
-        <f t="shared" si="2"/>
-        <v>9.0000000000000052E-2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.05</v>
+      </c>
+      <c r="K4" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="L4" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>-7</v>
       </c>
       <c r="B5">
-        <f t="shared" si="0"/>
-        <v>0.53</v>
+        <v>0.7</v>
       </c>
       <c r="C5">
-        <f t="shared" si="1"/>
-        <v>0.35999999999999988</v>
+        <v>0.2</v>
       </c>
       <c r="D5">
-        <f t="shared" si="2"/>
-        <v>0.11000000000000006</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.1</v>
+      </c>
+      <c r="K5" s="2">
+        <v>0.7</v>
+      </c>
+      <c r="L5" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>-6</v>
       </c>
       <c r="B6">
-        <f t="shared" si="0"/>
-        <v>0.49</v>
+        <v>0.6</v>
       </c>
       <c r="C6">
-        <f t="shared" si="1"/>
-        <v>0.37999999999999989</v>
+        <v>0.25</v>
       </c>
       <c r="D6">
-        <f t="shared" si="2"/>
-        <v>0.13000000000000006</v>
-      </c>
-      <c r="F6">
-        <v>81</v>
-      </c>
-      <c r="G6">
-        <v>80.2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.15</v>
+      </c>
+      <c r="K6" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="L6" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="M6" s="2">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>-5</v>
       </c>
       <c r="B7">
-        <f t="shared" si="0"/>
-        <v>0.45000000000000007</v>
+        <v>0.5</v>
       </c>
       <c r="C7">
-        <f t="shared" si="1"/>
-        <v>0.39999999999999991</v>
+        <v>0.3</v>
       </c>
       <c r="D7">
-        <f t="shared" si="2"/>
-        <v>0.15000000000000005</v>
-      </c>
-      <c r="G7">
-        <f>F6-G6</f>
-        <v>0.79999999999999716</v>
-      </c>
-      <c r="H7" t="b">
-        <f>IF(_xlfn.FLOOR.MATH(G7)=G7,"Can Use as key",IF(G7&gt;0,TRUE,FALSE))</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.2</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="L7" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>-4</v>
       </c>
       <c r="B8">
-        <f t="shared" si="0"/>
-        <v>0.41000000000000003</v>
+        <v>0.4</v>
       </c>
       <c r="C8">
-        <f t="shared" si="1"/>
-        <v>0.41999999999999993</v>
+        <v>0.35</v>
       </c>
       <c r="D8">
-        <f t="shared" si="2"/>
-        <v>0.17000000000000004</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.25</v>
+      </c>
+      <c r="K8" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="L8" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="M8" s="2">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>-3</v>
       </c>
       <c r="B9">
-        <f t="shared" si="0"/>
-        <v>0.37</v>
+        <v>0.3</v>
       </c>
       <c r="C9">
-        <f t="shared" si="1"/>
-        <v>0.43999999999999995</v>
+        <v>0.4</v>
       </c>
       <c r="D9">
-        <f t="shared" si="2"/>
-        <v>0.19000000000000003</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.3</v>
+      </c>
+      <c r="K9" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="L9" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="M9" s="2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>-2</v>
       </c>
       <c r="B10">
-        <f t="shared" si="0"/>
-        <v>0.33000000000000007</v>
+        <v>0.3</v>
       </c>
       <c r="C10">
-        <f t="shared" si="1"/>
-        <v>0.45999999999999996</v>
+        <v>0.4</v>
       </c>
       <c r="D10">
-        <f t="shared" si="2"/>
-        <v>0.21000000000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.3</v>
+      </c>
+      <c r="K10" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="L10" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="M10" s="2">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>-1</v>
       </c>
       <c r="B11">
-        <f>1-SUM(C11:D11)</f>
-        <v>0.29000000000000004</v>
+        <v>0.25</v>
       </c>
       <c r="C11">
-        <f t="shared" si="1"/>
-        <v>0.48</v>
+        <v>0.4</v>
       </c>
       <c r="D11">
-        <f t="shared" si="2"/>
-        <v>0.23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.35</v>
+      </c>
+      <c r="K11" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="L11" s="2">
+        <v>0.4</v>
+      </c>
+      <c r="M11" s="2">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>0</v>
       </c>
       <c r="B12">
-        <f>C12/2</f>
         <v>0.25</v>
       </c>
       <c r="C12">
-        <f>G1</f>
-        <v>0.5</v>
+        <v>0.35</v>
       </c>
       <c r="D12">
-        <f>C12/2</f>
+        <v>0.4</v>
+      </c>
+      <c r="K12" s="2">
         <v>0.25</v>
       </c>
-      <c r="G12">
-        <f>(G2)*G7</f>
-        <v>1.5999999999999945E-2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="L12" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="M12" s="2">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1</v>
       </c>
       <c r="B13">
-        <f t="shared" ref="B13:B22" si="3">B12-$G$2</f>
-        <v>0.23</v>
+        <v>0.2</v>
       </c>
       <c r="C13">
-        <f t="shared" ref="C13:C22" si="4">C12-($G$2)</f>
-        <v>0.48</v>
+        <v>0.35</v>
       </c>
       <c r="D13">
-        <f>1-SUM(B13:C13)</f>
-        <v>0.29000000000000004</v>
-      </c>
-      <c r="G13">
-        <f>IF(_xlfn.FLOOR.MATH($G$7)=$G$7,"Can Use as key",IF($G$7&gt;0,B12-$G$12,B12+$G$12))</f>
-        <v>0.23400000000000004</v>
-      </c>
-      <c r="H13">
-        <f>IF(_xlfn.FLOOR.MATH($G$7)=$G$7,"Can Use as key",IF($G$7&gt;0,C12-$G$12,C12+$G$12))</f>
-        <v>0.48400000000000004</v>
-      </c>
-      <c r="I13">
-        <f>IF(_xlfn.FLOOR.MATH($G$7)=$G$7,"Can Use as key",IF($G$7&gt;0,D12+$G$12,D12-$G$12))</f>
-        <v>0.26599999999999996</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.45</v>
+      </c>
+      <c r="K13" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="L13" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="M13" s="2">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2</v>
       </c>
       <c r="B14">
-        <f t="shared" si="3"/>
-        <v>0.21000000000000002</v>
+        <v>0.15</v>
       </c>
       <c r="C14">
-        <f t="shared" si="4"/>
-        <v>0.45999999999999996</v>
+        <v>0.3</v>
       </c>
       <c r="D14">
-        <f t="shared" ref="D14:D22" si="5">1-SUM(B14:C14)</f>
-        <v>0.33000000000000007</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="K14" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="L14" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="M14" s="2">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>3</v>
       </c>
       <c r="B15">
-        <f t="shared" si="3"/>
-        <v>0.19000000000000003</v>
+        <v>0.1</v>
       </c>
       <c r="C15">
-        <f t="shared" si="4"/>
-        <v>0.43999999999999995</v>
+        <v>0.3</v>
       </c>
       <c r="D15">
-        <f t="shared" si="5"/>
-        <v>0.37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+        <v>0.6</v>
+      </c>
+      <c r="K15" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="L15" s="2">
+        <v>0.3</v>
+      </c>
+      <c r="M15" s="2">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>4</v>
       </c>
       <c r="B16">
-        <f t="shared" si="3"/>
-        <v>0.17000000000000004</v>
+        <v>0.09</v>
       </c>
       <c r="C16">
-        <f t="shared" si="4"/>
-        <v>0.41999999999999993</v>
+        <v>0.25</v>
       </c>
       <c r="D16">
-        <f t="shared" si="5"/>
-        <v>0.41000000000000003</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.66</v>
+      </c>
+      <c r="K16" s="2">
+        <v>0.09</v>
+      </c>
+      <c r="L16" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="M16" s="2">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>5</v>
       </c>
       <c r="B17">
-        <f t="shared" si="3"/>
-        <v>0.15000000000000005</v>
+        <v>0.08</v>
       </c>
       <c r="C17">
-        <f t="shared" si="4"/>
-        <v>0.39999999999999991</v>
+        <v>0.2</v>
       </c>
       <c r="D17">
-        <f t="shared" si="5"/>
-        <v>0.45000000000000007</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.72</v>
+      </c>
+      <c r="K17" s="2">
+        <v>0.08</v>
+      </c>
+      <c r="L17" s="2">
+        <v>0.2</v>
+      </c>
+      <c r="M17" s="2">
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>6</v>
       </c>
       <c r="B18">
-        <f t="shared" si="3"/>
-        <v>0.13000000000000006</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="C18">
-        <f t="shared" si="4"/>
-        <v>0.37999999999999989</v>
+        <v>0.15</v>
       </c>
       <c r="D18">
-        <f t="shared" si="5"/>
-        <v>0.49</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.78</v>
+      </c>
+      <c r="K18" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L18" s="2">
+        <v>0.15</v>
+      </c>
+      <c r="M18" s="2">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>7</v>
       </c>
       <c r="B19">
-        <f t="shared" si="3"/>
-        <v>0.11000000000000006</v>
+        <v>0.06</v>
       </c>
       <c r="C19">
-        <f t="shared" si="4"/>
-        <v>0.35999999999999988</v>
+        <v>0.1</v>
       </c>
       <c r="D19">
-        <f t="shared" si="5"/>
-        <v>0.53</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.84</v>
+      </c>
+      <c r="K19" s="2">
+        <v>0.06</v>
+      </c>
+      <c r="L19" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="M19" s="2">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>8</v>
       </c>
       <c r="B20">
-        <f t="shared" si="3"/>
-        <v>9.0000000000000052E-2</v>
+        <f t="shared" ref="B13:B22" si="3">B19-$G$2</f>
+        <v>3.9999999999999994E-2</v>
       </c>
       <c r="C20">
-        <f t="shared" si="4"/>
-        <v>0.33999999999999986</v>
+        <f t="shared" ref="C13:C22" si="4">C19-($G$2)</f>
+        <v>0.08</v>
       </c>
       <c r="D20">
-        <f t="shared" si="5"/>
-        <v>0.57000000000000006</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" ref="D14:D22" si="5">1-SUM(B20:C20)</f>
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>9</v>
       </c>
       <c r="B21">
         <f t="shared" si="3"/>
-        <v>7.0000000000000048E-2</v>
+        <v>1.9999999999999993E-2</v>
       </c>
       <c r="C21">
         <f t="shared" si="4"/>
-        <v>0.31999999999999984</v>
+        <v>0.06</v>
       </c>
       <c r="D21">
         <f t="shared" si="5"/>
-        <v>0.6100000000000001</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>10</v>
       </c>
       <c r="B22">
         <f t="shared" si="3"/>
-        <v>5.0000000000000044E-2</v>
+        <v>0</v>
       </c>
       <c r="C22">
         <f t="shared" si="4"/>
-        <v>0.29999999999999982</v>
+        <v>3.9999999999999994E-2</v>
       </c>
       <c r="D22">
         <f t="shared" si="5"/>
-        <v>0.65000000000000013</v>
+        <v>0.96</v>
       </c>
     </row>
   </sheetData>

</xml_diff>